<commit_message>
add data dictionaries as R data objects #18
</commit_message>
<xml_diff>
--- a/inst/docs/diccionario-variables-replicas.xlsx
+++ b/inst/docs/diccionario-variables-replicas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariagargiulo/HRDAG/verdata/inst/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED286A8-DDC6-7546-9F2C-814C7C864C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DDFAF7-CDBC-6748-87F9-1D8147B053A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario_replicas" sheetId="1" r:id="rId1"/>
@@ -65,10 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">Variable dicotómica que toma el valor de = 1 cuando la víctima aparece en esta fuente, = 0 en caso contrario </t>
-  </si>
-  <si>
-    <t>1 
-0</t>
   </si>
   <si>
     <t>in_2</t>
@@ -223,11 +219,6 @@
     <t>edad_jep</t>
   </si>
   <si>
-    <t>0 a 15 años: "INFANCIA",
-        14 a 17 años: "ADOLESCENCIA",
-          edad igual o mayor a 18 años: "ADULTEZ"</t>
-  </si>
-  <si>
     <t>edad_jep_imputed</t>
   </si>
   <si>
@@ -235,12 +226,6 @@
   </si>
   <si>
     <t>Variable nominal que clasifica la etnia de la víctima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDIGENA
- MESTIZO
- NARP (Población Negra, Afrocolombiana, Raizal y Palenquera) 
-  ROM </t>
   </si>
   <si>
     <t>etnia_imputed</t>
@@ -285,15 +270,6 @@
     <t>Variable nominal que clasifica el responsable de los hechos.</t>
   </si>
   <si>
-    <t xml:space="preserve"> EST: Agentes del Estado    
-GUE-ELN: Guerrilla ELN
-GUE-FARC: Guerrilla FARC-EP 
-GUE-OTRO: Guerrilla otra
-multiple: Múltiples actores
-OTRO: Otro     
-PARA: Paramilitares</t>
-  </si>
-  <si>
     <t>p_str_imputed</t>
   </si>
   <si>
@@ -312,12 +288,6 @@
     <t xml:space="preserve">Año del hecho </t>
   </si>
   <si>
-    <t>Reclutamiento: 1990-2017
-Homicidio: 1985-2018
-Desaparición: 1985-2016
-Secuestro: 1990-2018</t>
-  </si>
-  <si>
     <t>yymm_hecho</t>
   </si>
   <si>
@@ -330,10 +300,6 @@
     <t>Variable nominal que clasifica y/o agrupa la etnia de la víctima. Variable para reclutamiento.</t>
   </si>
   <si>
-    <t>ETNICO: indígena, NARP y ROM
-MESTIZO: Mestizo</t>
-  </si>
-  <si>
     <t>etnia2_imputed</t>
   </si>
   <si>
@@ -344,10 +310,6 @@
   </si>
   <si>
     <t>Variable nominal que agrupa en rangos de edad (edad_jep) la edad de la víctima al momento de los hechos.</t>
-  </si>
-  <si>
-    <t>MENOR: Infancia, adolescencia.
-ADULTO: adultez</t>
   </si>
   <si>
     <t>edad_minors_imputed</t>
@@ -375,18 +337,6 @@
   </si>
   <si>
     <t>Variable nominal que muestan las macrorregiones definidas por la CEV.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Amazonía" ,
- "Antioquia-Eje Cafetero" 
-"Bogotá",
-"Caribe e Insular" , 
-"Centro Andino",
-"Magdalena Medio",
- "Nororiente",
-"Orinoquía",
-"Pacífico",
-"Sur Andina" </t>
   </si>
   <si>
     <t>is_conflict_dis</t>
@@ -425,16 +375,66 @@
     <t>region</t>
   </si>
   <si>
-    <t>Variable nominal que muestra la información de los municipios que conforman la "zona de distensión", los municipios vecinos de dicho territorio, así como en el resto de los municipios de Colombia.</t>
+    <t>0 a 15 años: INFANCIA,
+        14 a 17 años: ADOLESCENCIA,
+          edad igual o mayor a 18 años: ADULTEZ</t>
   </si>
   <si>
-    <t xml:space="preserve">"Resto del país",
- "Cercano zona desmilitarizada",
-"Municipio desmilitarizado" </t>
+    <t xml:space="preserve">INDIGENA,
+ MESTIZO,
+ NARP (Población Negra, Afrocolombiana, Raizal y Palenquera), 
+  ROM </t>
   </si>
   <si>
-    <t>HOMBRE
+    <t xml:space="preserve"> EST: Agentes del Estado,    
+GUE-ELN: Guerrilla ELN,
+GUE-FARC: Guerrilla FARC-EP, 
+GUE-OTRO: Guerrilla otra,
+multiple: Múltiples actores,
+OTRO: Otro,     
+PARA: Paramilitares,</t>
+  </si>
+  <si>
+    <t>HOMBRE,
 MUJER</t>
+  </si>
+  <si>
+    <t>Reclutamiento: 1990-2017,
+Homicidio: 1985-2018,
+Desaparición: 1985-2016,
+Secuestro: 1990-2018,</t>
+  </si>
+  <si>
+    <t>1, 
+0</t>
+  </si>
+  <si>
+    <t>ETNICO: indígena, NARP y ROM;
+MESTIZO: Mestizo</t>
+  </si>
+  <si>
+    <t>MENOR: Infancia, adolescencia;
+ADULTO: adultez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resto del país,
+ Cercano zona desmilitarizada,
+Municipio desmilitarizado </t>
+  </si>
+  <si>
+    <t>Variable nominal que muestra la información de los municipios que conforman la 'zona de distensión', los municipios vecinos de dicho territorio, así como en el resto de los municipios de Colombia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amazonía,
+ Antioquia-Eje Cafetero, 
+Bogotá,
+Caribe e Insular, 
+Centro Andino,
+Magdalena Medio,
+ Nororiente,
+Orinoquía,
+Pacífico,
+Sur Andina </t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
   </sheetPr>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -911,7 +911,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
@@ -938,7 +938,7 @@
     </row>
     <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
@@ -947,7 +947,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="7"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -983,7 +983,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="7"/>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="7"/>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="8" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
@@ -1055,7 +1055,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="7"/>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="9" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
@@ -1091,7 +1091,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="7"/>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="10" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
@@ -1127,7 +1127,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="7"/>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="11" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
@@ -1163,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="7"/>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="12" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -1199,7 +1199,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="13" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -1235,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="7"/>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="14" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -1271,7 +1271,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="7"/>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="15" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
@@ -1307,7 +1307,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="7"/>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="16" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
@@ -1343,7 +1343,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7"/>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="17" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -1379,7 +1379,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="7"/>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="18" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
@@ -1415,7 +1415,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="7"/>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="19" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>11</v>
@@ -1451,7 +1451,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="7"/>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="20" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>11</v>
@@ -1487,7 +1487,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="7"/>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="21" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>11</v>
@@ -1523,7 +1523,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="7"/>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="22" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="7"/>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="23" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
@@ -1595,7 +1595,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="7"/>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="24" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
@@ -1631,7 +1631,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="7"/>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="25" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>11</v>
@@ -1667,7 +1667,7 @@
         <v>12</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="7"/>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="26" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>11</v>
@@ -1703,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="7"/>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="27" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>11</v>
@@ -1739,7 +1739,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="28" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>11</v>
@@ -1775,7 +1775,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="29" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
@@ -1811,7 +1811,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="30" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>11</v>
@@ -1847,7 +1847,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="7"/>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="31" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
@@ -1883,7 +1883,7 @@
         <v>12</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="7"/>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="32" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>11</v>
@@ -1919,7 +1919,7 @@
         <v>12</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="7"/>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="33" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>11</v>
@@ -1955,7 +1955,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="7"/>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="34" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>11</v>
@@ -1991,7 +1991,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="7"/>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="35" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>11</v>
@@ -2027,7 +2027,7 @@
         <v>12</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="7"/>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="36" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>11</v>
@@ -2063,7 +2063,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="7"/>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="37" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>11</v>
@@ -2099,7 +2099,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="7"/>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="38" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="7"/>
@@ -2162,16 +2162,16 @@
     </row>
     <row r="39" spans="1:26" ht="340" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="7"/>
@@ -2198,16 +2198,16 @@
     </row>
     <row r="40" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="7"/>
@@ -2234,16 +2234,16 @@
     </row>
     <row r="41" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="7"/>
@@ -2270,16 +2270,16 @@
     </row>
     <row r="42" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
@@ -2306,16 +2306,16 @@
     </row>
     <row r="43" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="7"/>
@@ -2342,16 +2342,16 @@
     </row>
     <row r="44" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="7"/>
@@ -2378,16 +2378,16 @@
     </row>
     <row r="45" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="7"/>
@@ -2414,16 +2414,16 @@
     </row>
     <row r="46" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="7"/>
@@ -2450,16 +2450,16 @@
     </row>
     <row r="47" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="7"/>
@@ -2486,16 +2486,16 @@
     </row>
     <row r="48" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="7"/>
@@ -2522,16 +2522,16 @@
     </row>
     <row r="49" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="7"/>
@@ -2558,16 +2558,16 @@
     </row>
     <row r="50" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="7"/>
@@ -2594,16 +2594,16 @@
     </row>
     <row r="51" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="7"/>
@@ -2630,16 +2630,16 @@
     </row>
     <row r="52" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="7"/>
@@ -2666,16 +2666,16 @@
     </row>
     <row r="53" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="7"/>
@@ -2702,16 +2702,16 @@
     </row>
     <row r="54" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="7"/>
@@ -2738,16 +2738,16 @@
     </row>
     <row r="55" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="7"/>
@@ -2774,16 +2774,16 @@
     </row>
     <row r="56" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="7"/>
@@ -29141,8 +29141,8 @@
   </sheetPr>
   <dimension ref="A1:D1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29169,156 +29169,156 @@
     </row>
     <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="170" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="136" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="119" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">

</xml_diff>